<commit_message>
Minor UI enahncements (background image) and some experiemnt data updates from ali
</commit_message>
<xml_diff>
--- a/Excel/Configurations.xlsx
+++ b/Excel/Configurations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damma\Documents\Fall2024\Master'sProject\BloodResearch\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B8BE67D-A74F-45C5-A9D3-D6DC60A188FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5533882A-D7ED-4AB7-8E31-E20E34E40B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6EBC93B0-168C-4993-800D-5FF6FD59B923}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Incubation Time (hrs)</t>
   </si>
@@ -63,6 +63,36 @@
   </si>
   <si>
     <t>Arginine (mM)</t>
+  </si>
+  <si>
+    <t>Scores</t>
+  </si>
+  <si>
+    <t>0.732,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.845,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.393,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.684,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.914,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.927,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        0.641,</t>
+  </si>
+  <si>
+    <t>Generation 2:</t>
+  </si>
+  <si>
+    <t>Generation 3:</t>
   </si>
 </sst>
 </file>
@@ -105,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -113,11 +143,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -125,14 +185,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -405,6 +471,31 @@
       </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -419,18 +510,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{412C692F-8409-4C61-BCA6-24655B07CB29}" name="Table2" displayName="Table2" ref="B1:J9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="B1:J9" xr:uid="{412C692F-8409-4C61-BCA6-24655B07CB29}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{700097B1-2C5C-47AB-B7EB-D454039ACA18}" name="Incubation Time (hrs)" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{F6391EA8-3C8F-4FBE-B58D-9E6F10FD1DFA}" name="Concentration of methyl alpha glucopyranoside (M)" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{3E6969CD-68D0-4455-AC59-EB313924304A}" name="pH" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{FEDEDC17-C854-4437-8C93-662A31A8C3F2}" name="6 kda dextran (% w/v)" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{604FAC36-EF22-438C-B176-C35E21D9E62F}" name="Trehalose (M)" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4D2DD98F-9F7F-446B-9541-716B25195B1B}" name="EGCG (% w/v)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{EFB30265-53BB-42C9-AD01-0E70B896E7B4}" name="Polaxamer 188 (% w/v)" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{4A3BE25E-BAB5-4347-970D-52DE57C1D292}" name="BSA (% w/v)" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{0026819D-D328-4517-88D2-723C7EBE90D0}" name="Arginine (mM)" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{412C692F-8409-4C61-BCA6-24655B07CB29}" name="Table2" displayName="Table2" ref="B1:K9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="B1:K9" xr:uid="{412C692F-8409-4C61-BCA6-24655B07CB29}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{700097B1-2C5C-47AB-B7EB-D454039ACA18}" name="Incubation Time (hrs)" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{F6391EA8-3C8F-4FBE-B58D-9E6F10FD1DFA}" name="Concentration of methyl alpha glucopyranoside (M)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{3E6969CD-68D0-4455-AC59-EB313924304A}" name="pH" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{FEDEDC17-C854-4437-8C93-662A31A8C3F2}" name="6 kda dextran (% w/v)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{604FAC36-EF22-438C-B176-C35E21D9E62F}" name="Trehalose (M)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4D2DD98F-9F7F-446B-9541-716B25195B1B}" name="EGCG (% w/v)" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{EFB30265-53BB-42C9-AD01-0E70B896E7B4}" name="Polaxamer 188 (% w/v)" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{4A3BE25E-BAB5-4347-970D-52DE57C1D292}" name="BSA (% w/v)" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{0026819D-D328-4517-88D2-723C7EBE90D0}" name="Arginine (mM)" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{A29FDEA6-5034-4804-9FD2-4990BCDE7A3E}" name="Scores" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -753,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB25009C-2C31-4785-8C4E-9F346F0BDE00}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="62" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="A21" activeCellId="1" sqref="A16:XFD16 A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,9 +862,10 @@
     <col min="8" max="8" width="24.36328125" customWidth="1"/>
     <col min="9" max="9" width="14.1796875" customWidth="1"/>
     <col min="10" max="10" width="16.54296875" customWidth="1"/>
+    <col min="11" max="11" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="132" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,8 +893,11 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2">
         <v>7</v>
@@ -830,8 +926,11 @@
       <c r="J2" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2">
         <v>0</v>
@@ -860,8 +959,11 @@
       <c r="J3" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="2">
         <v>3</v>
@@ -890,8 +992,11 @@
       <c r="J4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="K4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
         <v>7</v>
@@ -920,8 +1025,11 @@
       <c r="J5" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="K5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>7</v>
@@ -950,8 +1058,11 @@
       <c r="J6" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="K6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="2">
         <v>0</v>
@@ -980,8 +1091,11 @@
       <c r="J7" s="2">
         <v>250</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="K7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>0</v>
@@ -1010,8 +1124,11 @@
       <c r="J8" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="K8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="2">
         <v>7</v>
@@ -1039,6 +1156,827 @@
       </c>
       <c r="J9" s="2">
         <v>150</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.73599999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5.6</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J14" s="4">
+        <v>300</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="D15" s="4">
+        <v>6.8</v>
+      </c>
+      <c r="E15" s="4">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="J15" s="4">
+        <v>300</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D16" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="E16" s="4">
+        <v>30</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D17" s="4">
+        <v>7</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="J17" s="4">
+        <v>100</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>7</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="E18" s="4">
+        <v>18</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>7</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5.6</v>
+      </c>
+      <c r="E19" s="4">
+        <v>18</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="J19" s="4">
+        <v>300</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>7</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D20" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="E20" s="4">
+        <v>4</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="J20" s="4">
+        <v>200</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4">
+        <v>28</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="J21" s="4">
+        <v>200</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D26" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="E26" s="4">
+        <v>20</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D27" s="4">
+        <v>7</v>
+      </c>
+      <c r="E27" s="4">
+        <v>4</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>2</v>
+      </c>
+      <c r="I27" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>7</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>7</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="J28" s="4">
+        <v>200</v>
+      </c>
+      <c r="K28" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>7</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>5</v>
+      </c>
+      <c r="E29" s="4">
+        <v>18</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="J29" s="4">
+        <v>100</v>
+      </c>
+      <c r="K29" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D30" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="E30" s="4">
+        <v>4</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="J30" s="4">
+        <v>200</v>
+      </c>
+      <c r="K30" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>7</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="E31" s="4">
+        <v>18</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="J31" s="4">
+        <v>300</v>
+      </c>
+      <c r="K31" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5</v>
+      </c>
+      <c r="E32" s="4">
+        <v>18</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="J32" s="4">
+        <v>200</v>
+      </c>
+      <c r="K32" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I33" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="J33" s="4">
+        <v>300</v>
+      </c>
+      <c r="K33" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E47" s="2">
+        <v>6.6</v>
+      </c>
+      <c r="F47" s="2">
+        <v>20</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="K47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E48" s="2">
+        <v>7</v>
+      </c>
+      <c r="F48" s="2">
+        <v>4</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <v>2</v>
+      </c>
+      <c r="J48" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="K48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="C49" s="2">
+        <v>7</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2">
+        <v>7</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I49" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K49" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="C50" s="2">
+        <v>7</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E50" s="2">
+        <v>5</v>
+      </c>
+      <c r="F50" s="2">
+        <v>18</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="H50" s="2">
+        <v>1</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="J50" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="K50" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="C51" s="2">
+        <v>7</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E51" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="F51" s="2">
+        <v>4</v>
+      </c>
+      <c r="G51" s="2">
+        <v>1</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0</v>
+      </c>
+      <c r="I51" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="J51" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="K51" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="C52" s="2">
+        <v>7</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E52" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="F52" s="2">
+        <v>18</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="J52" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="K52" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="C53" s="2">
+        <v>0</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E53" s="2">
+        <v>5</v>
+      </c>
+      <c r="F53" s="2">
+        <v>18</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="K53" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="C54" s="2">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E54" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0</v>
+      </c>
+      <c r="G54" s="2">
+        <v>1</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J54" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="K54" s="2">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented FetchExperiments through api gateway/aws lambda to now be able to "View Experiments" that the user has saved
</commit_message>
<xml_diff>
--- a/Excel/Configurations.xlsx
+++ b/Excel/Configurations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damma\Documents\Fall2024\Master'sProject\BloodResearch\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5533882A-D7ED-4AB7-8E31-E20E34E40B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFB8860-4256-449A-9CA1-66B0F3A656B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6EBC93B0-168C-4993-800D-5FF6FD59B923}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>Incubation Time (hrs)</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Generation 3:</t>
+  </si>
+  <si>
+    <t>Generation 4:</t>
   </si>
 </sst>
 </file>
@@ -177,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -189,6 +192,9 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -847,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB25009C-2C31-4785-8C4E-9F346F0BDE00}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="62" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="A21" activeCellId="1" sqref="A16:XFD16 A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="71" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1520,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="4">
-        <v>999</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
@@ -1552,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="4">
-        <v>999</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="28" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
@@ -1584,7 +1590,7 @@
         <v>200</v>
       </c>
       <c r="K28" s="4">
-        <v>999</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="29" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
@@ -1616,7 +1622,7 @@
         <v>100</v>
       </c>
       <c r="K29" s="4">
-        <v>999</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
@@ -1648,7 +1654,7 @@
         <v>200</v>
       </c>
       <c r="K30" s="4">
-        <v>999</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="31" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
@@ -1680,7 +1686,7 @@
         <v>300</v>
       </c>
       <c r="K31" s="4">
-        <v>999</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="32" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
@@ -1712,7 +1718,7 @@
         <v>200</v>
       </c>
       <c r="K32" s="4">
-        <v>999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
@@ -1744,240 +1750,389 @@
         <v>300</v>
       </c>
       <c r="K33" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="4">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="D39" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="E39" s="4">
+        <v>18</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="J39" s="4">
+        <v>300</v>
+      </c>
+      <c r="K39" s="4">
         <v>999</v>
       </c>
     </row>
+    <row r="40" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="4">
+        <v>7</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D40" s="4">
+        <v>7</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>1</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="I40" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="J40" s="4">
+        <v>300</v>
+      </c>
+      <c r="K40" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B41" s="4">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D41" s="4">
+        <v>5</v>
+      </c>
+      <c r="E41" s="4">
+        <v>12</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="J41" s="4">
+        <v>300</v>
+      </c>
+      <c r="K41" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B42" s="4">
+        <v>7</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D42" s="4">
+        <v>7</v>
+      </c>
+      <c r="E42" s="4">
+        <v>14</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="J42" s="4">
+        <v>300</v>
+      </c>
+      <c r="K42" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B43" s="4">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="D43" s="4">
+        <v>7</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4">
+        <v>1</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="I43" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="J43" s="4">
+        <v>200</v>
+      </c>
+      <c r="K43" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D44" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="E44" s="4">
+        <v>20</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1</v>
+      </c>
+      <c r="I44" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="J44" s="4">
+        <v>150</v>
+      </c>
+      <c r="K44" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B45" s="4">
+        <v>7</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D45" s="4">
+        <v>7</v>
+      </c>
+      <c r="E45" s="4">
+        <v>4</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H45" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="J45" s="4">
+        <v>0</v>
+      </c>
+      <c r="K45" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D46" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="E46" s="4">
+        <v>30</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="J46" s="4">
+        <v>300</v>
+      </c>
+      <c r="K46" s="4">
+        <v>999</v>
+      </c>
+    </row>
     <row r="47" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C47" s="2">
-        <v>0</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="E47" s="2">
-        <v>6.6</v>
-      </c>
-      <c r="F47" s="2">
-        <v>20</v>
-      </c>
-      <c r="G47" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H47" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="I47" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="J47" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="K47" s="2">
-        <v>0</v>
-      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
     </row>
     <row r="48" spans="2:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C48" s="2">
-        <v>0</v>
-      </c>
-      <c r="D48" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="E48" s="2">
-        <v>7</v>
-      </c>
-      <c r="F48" s="2">
-        <v>4</v>
-      </c>
-      <c r="G48" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="H48" s="2">
-        <v>0</v>
-      </c>
-      <c r="I48" s="2">
-        <v>2</v>
-      </c>
-      <c r="J48" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="K48" s="2">
-        <v>0</v>
-      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
     </row>
     <row r="49" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C49" s="2">
-        <v>7</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2">
-        <v>7</v>
-      </c>
-      <c r="F49" s="2">
-        <v>0</v>
-      </c>
-      <c r="G49" s="2">
-        <v>1</v>
-      </c>
-      <c r="H49" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I49" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="J49" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="K49" s="2">
-        <v>200</v>
-      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
     </row>
     <row r="50" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C50" s="2">
-        <v>7</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="E50" s="2">
-        <v>5</v>
-      </c>
-      <c r="F50" s="2">
-        <v>18</v>
-      </c>
-      <c r="G50" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="H50" s="2">
-        <v>1</v>
-      </c>
-      <c r="I50" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="J50" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="K50" s="2">
-        <v>100</v>
-      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
     </row>
     <row r="51" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C51" s="2">
-        <v>7</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="E51" s="2">
-        <v>5.4</v>
-      </c>
-      <c r="F51" s="2">
-        <v>4</v>
-      </c>
-      <c r="G51" s="2">
-        <v>1</v>
-      </c>
-      <c r="H51" s="2">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="J51" s="2">
-        <v>1.9</v>
-      </c>
-      <c r="K51" s="2">
-        <v>200</v>
-      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
     </row>
     <row r="52" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C52" s="2">
-        <v>7</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="E52" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="F52" s="2">
-        <v>18</v>
-      </c>
-      <c r="G52" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H52" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="I52" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="J52" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="K52" s="2">
-        <v>300</v>
-      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
     </row>
     <row r="53" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C53" s="2">
-        <v>0</v>
-      </c>
-      <c r="D53" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="E53" s="2">
-        <v>5</v>
-      </c>
-      <c r="F53" s="2">
-        <v>18</v>
-      </c>
-      <c r="G53" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="H53" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="I53" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J53" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="K53" s="2">
-        <v>200</v>
-      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
     </row>
     <row r="54" spans="3:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C54" s="2">
-        <v>0</v>
-      </c>
-      <c r="D54" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E54" s="2">
-        <v>5.8</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0</v>
-      </c>
-      <c r="G54" s="2">
-        <v>1</v>
-      </c>
-      <c r="H54" s="2">
-        <v>0</v>
-      </c>
-      <c r="I54" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="J54" s="2">
-        <v>1.9</v>
-      </c>
-      <c r="K54" s="2">
-        <v>300</v>
-      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>